<commit_message>
lots of temp data converted to spreadsheets from HOBO files
</commit_message>
<xml_diff>
--- a/Data/20170408_Sampling-Data.xlsx
+++ b/Data/20170408_Sampling-Data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sample Key" sheetId="1" r:id="rId1"/>
     <sheet name="Morts" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Sample Key'!$2:$2</definedName>
@@ -1317,8 +1318,8 @@
   <dimension ref="A1:I165"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A56" sqref="A56:XFD56"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -3365,7 +3366,9 @@
       <c r="B105" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C105" s="3"/>
+      <c r="C105" s="3">
+        <v>1</v>
+      </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -3446,7 +3449,9 @@
       <c r="B114" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C114" s="3"/>
+      <c r="C114" s="3">
+        <v>2</v>
+      </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
@@ -3527,7 +3532,9 @@
       <c r="B123" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C123" s="3"/>
+      <c r="C123" s="3">
+        <v>3</v>
+      </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
@@ -3608,7 +3615,9 @@
       <c r="B132" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C132" s="3"/>
+      <c r="C132" s="3">
+        <v>4</v>
+      </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
@@ -3689,7 +3698,9 @@
       <c r="B142" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C142" s="3"/>
+      <c r="C142" s="3">
+        <v>5</v>
+      </c>
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
@@ -5041,6 +5052,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
     <mergeCell ref="I35:I37"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="I20:I22"/>
@@ -5048,12 +5065,6 @@
     <mergeCell ref="I26:I28"/>
     <mergeCell ref="I29:I31"/>
     <mergeCell ref="I32:I34"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5063,4 +5074,23 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated larval data and references
</commit_message>
<xml_diff>
--- a/Data/20170408_Sampling-Data.xlsx
+++ b/Data/20170408_Sampling-Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="0" windowWidth="25500" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="9160" yWindow="240" windowWidth="16440" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Key" sheetId="1" r:id="rId1"/>
@@ -1318,8 +1318,8 @@
   <dimension ref="A1:I165"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -3875,10 +3875,9 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="5" ySplit="15" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1:M8"/>
+      <pane xSplit="11440" topLeftCell="J1" activePane="topRight"/>
+      <selection activeCell="B33" sqref="B33"/>
+      <selection pane="topRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5052,6 +5051,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
     <mergeCell ref="I35:I37"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="I20:I22"/>
@@ -5059,12 +5064,6 @@
     <mergeCell ref="I26:I28"/>
     <mergeCell ref="I29:I31"/>
     <mergeCell ref="I32:I34"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
updated files after the big spill
</commit_message>
<xml_diff>
--- a/Data/20170408_Sampling-Data.xlsx
+++ b/Data/20170408_Sampling-Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28331"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="11400" yWindow="0" windowWidth="13780" windowHeight="15440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sample Key" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="196">
   <si>
     <t>Notes</t>
   </si>
@@ -715,7 +715,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -849,6 +849,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -891,7 +899,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="143">
     <cellStyle name="Comma" xfId="132" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -959,6 +967,10 @@
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1025,6 +1037,10 @@
     <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="35" builtinId="5"/>
   </cellStyles>
@@ -1358,8 +1374,8 @@
   <dimension ref="A1:J165"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -3443,493 +3459,798 @@
       </c>
     </row>
     <row r="105" spans="2:7">
+      <c r="B105" s="6">
+        <v>43203</v>
+      </c>
       <c r="C105" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D105" s="3">
-        <v>1</v>
+      <c r="D105" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="14"/>
       <c r="G105" s="3"/>
     </row>
     <row r="106" spans="2:7">
+      <c r="B106" s="6">
+        <v>43203</v>
+      </c>
       <c r="C106" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D106" s="3"/>
+      <c r="D106" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E106" s="3"/>
       <c r="F106" s="14"/>
       <c r="G106" s="3"/>
     </row>
     <row r="107" spans="2:7">
+      <c r="B107" s="6">
+        <v>43203</v>
+      </c>
       <c r="C107" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D107" s="3"/>
+      <c r="D107" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E107" s="3"/>
       <c r="F107" s="14"/>
       <c r="G107" s="3"/>
     </row>
     <row r="108" spans="2:7">
+      <c r="B108" s="6">
+        <v>43203</v>
+      </c>
       <c r="C108" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="14"/>
       <c r="G108" s="3"/>
     </row>
     <row r="109" spans="2:7">
+      <c r="B109" s="6">
+        <v>43203</v>
+      </c>
       <c r="C109" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D109" s="3"/>
+      <c r="D109" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E109" s="3"/>
       <c r="F109" s="14"/>
       <c r="G109" s="3"/>
     </row>
     <row r="110" spans="2:7">
+      <c r="B110" s="6">
+        <v>43203</v>
+      </c>
       <c r="C110" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D110" s="3"/>
+      <c r="D110" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E110" s="3"/>
       <c r="F110" s="14"/>
       <c r="G110" s="3"/>
     </row>
     <row r="111" spans="2:7">
+      <c r="B111" s="6">
+        <v>43203</v>
+      </c>
       <c r="C111" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D111" s="3"/>
+      <c r="D111" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E111" s="3"/>
       <c r="F111" s="14"/>
       <c r="G111" s="3"/>
     </row>
     <row r="112" spans="2:7">
+      <c r="B112" s="6">
+        <v>43203</v>
+      </c>
       <c r="C112" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D112" s="3"/>
+      <c r="D112" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E112" s="3"/>
       <c r="F112" s="14"/>
       <c r="G112" s="3"/>
     </row>
-    <row r="113" spans="3:7">
+    <row r="113" spans="2:7">
+      <c r="B113" s="6">
+        <v>43203</v>
+      </c>
       <c r="C113" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E113" s="3"/>
       <c r="F113" s="14"/>
       <c r="G113" s="3"/>
     </row>
-    <row r="114" spans="3:7">
+    <row r="114" spans="2:7">
+      <c r="B114" s="6">
+        <v>43203</v>
+      </c>
       <c r="C114" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D114" s="3">
-        <v>2</v>
+      <c r="D114" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E114" s="3"/>
       <c r="F114" s="14"/>
       <c r="G114" s="3"/>
     </row>
-    <row r="115" spans="3:7">
+    <row r="115" spans="2:7">
+      <c r="B115" s="6">
+        <v>43203</v>
+      </c>
       <c r="C115" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D115" s="3"/>
+      <c r="D115" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E115" s="3"/>
       <c r="F115" s="14"/>
       <c r="G115" s="3"/>
     </row>
-    <row r="116" spans="3:7">
+    <row r="116" spans="2:7">
+      <c r="B116" s="6">
+        <v>43203</v>
+      </c>
       <c r="C116" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D116" s="3"/>
+      <c r="D116" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E116" s="3"/>
       <c r="F116" s="14"/>
       <c r="G116" s="3"/>
     </row>
-    <row r="117" spans="3:7">
+    <row r="117" spans="2:7">
+      <c r="B117" s="6">
+        <v>43203</v>
+      </c>
       <c r="C117" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D117" s="3"/>
+      <c r="D117" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E117" s="3"/>
       <c r="F117" s="14"/>
       <c r="G117" s="3"/>
     </row>
-    <row r="118" spans="3:7">
+    <row r="118" spans="2:7">
+      <c r="B118" s="6">
+        <v>43203</v>
+      </c>
       <c r="C118" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D118" s="3"/>
+      <c r="D118" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E118" s="3"/>
       <c r="F118" s="14"/>
       <c r="G118" s="3"/>
     </row>
-    <row r="119" spans="3:7">
+    <row r="119" spans="2:7">
+      <c r="B119" s="6">
+        <v>43203</v>
+      </c>
       <c r="C119" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D119" s="3"/>
+      <c r="D119" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E119" s="3"/>
       <c r="F119" s="14"/>
       <c r="G119" s="3"/>
     </row>
-    <row r="120" spans="3:7">
+    <row r="120" spans="2:7">
+      <c r="B120" s="6">
+        <v>43203</v>
+      </c>
       <c r="C120" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D120" s="3"/>
+      <c r="D120" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E120" s="3"/>
       <c r="F120" s="14"/>
       <c r="G120" s="3"/>
     </row>
-    <row r="121" spans="3:7">
+    <row r="121" spans="2:7">
+      <c r="B121" s="6">
+        <v>43203</v>
+      </c>
       <c r="C121" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E121" s="3"/>
       <c r="F121" s="14"/>
       <c r="G121" s="3"/>
     </row>
-    <row r="122" spans="3:7">
+    <row r="122" spans="2:7">
+      <c r="B122" s="6">
+        <v>43203</v>
+      </c>
       <c r="C122" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D122" s="3"/>
+      <c r="D122" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E122" s="3"/>
       <c r="F122" s="14"/>
       <c r="G122" s="3"/>
     </row>
-    <row r="123" spans="3:7">
+    <row r="123" spans="2:7">
+      <c r="B123" s="6">
+        <v>43203</v>
+      </c>
       <c r="C123" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D123" s="3">
-        <v>3</v>
+      <c r="D123" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="E123" s="3"/>
       <c r="F123" s="14"/>
       <c r="G123" s="3"/>
     </row>
-    <row r="124" spans="3:7">
+    <row r="124" spans="2:7">
+      <c r="B124" s="6">
+        <v>43203</v>
+      </c>
       <c r="C124" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E124" s="3"/>
       <c r="F124" s="14"/>
       <c r="G124" s="3"/>
     </row>
-    <row r="125" spans="3:7">
+    <row r="125" spans="2:7">
+      <c r="B125" s="6">
+        <v>43203</v>
+      </c>
       <c r="C125" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D125" s="3"/>
+      <c r="D125" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E125" s="3"/>
       <c r="F125" s="14"/>
       <c r="G125" s="3"/>
     </row>
-    <row r="126" spans="3:7">
+    <row r="126" spans="2:7">
+      <c r="B126" s="6">
+        <v>43203</v>
+      </c>
       <c r="C126" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D126" s="3"/>
+      <c r="D126" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E126" s="3"/>
       <c r="F126" s="14"/>
       <c r="G126" s="3"/>
     </row>
-    <row r="127" spans="3:7">
+    <row r="127" spans="2:7">
+      <c r="B127" s="6">
+        <v>43203</v>
+      </c>
       <c r="C127" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D127" s="3"/>
+      <c r="D127" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E127" s="3"/>
       <c r="F127" s="14"/>
       <c r="G127" s="3"/>
     </row>
-    <row r="128" spans="3:7">
+    <row r="128" spans="2:7">
+      <c r="B128" s="6">
+        <v>43203</v>
+      </c>
       <c r="C128" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D128" s="3"/>
+      <c r="D128" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E128" s="3"/>
       <c r="F128" s="14"/>
       <c r="G128" s="3"/>
     </row>
-    <row r="129" spans="3:7">
+    <row r="129" spans="2:7">
+      <c r="B129" s="6">
+        <v>43203</v>
+      </c>
       <c r="C129" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D129" s="3"/>
+      <c r="D129" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E129" s="3"/>
       <c r="F129" s="14"/>
       <c r="G129" s="3"/>
     </row>
-    <row r="130" spans="3:7">
+    <row r="130" spans="2:7">
+      <c r="B130" s="6">
+        <v>43203</v>
+      </c>
       <c r="C130" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D130" s="3"/>
+      <c r="D130" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E130" s="3"/>
       <c r="F130" s="14"/>
       <c r="G130" s="3"/>
     </row>
-    <row r="131" spans="3:7">
+    <row r="131" spans="2:7">
+      <c r="B131" s="6">
+        <v>43203</v>
+      </c>
       <c r="C131" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="D131" s="3"/>
+      <c r="D131" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E131" s="3"/>
       <c r="F131" s="14"/>
       <c r="G131" s="3"/>
     </row>
-    <row r="132" spans="3:7">
+    <row r="132" spans="2:7">
+      <c r="B132" s="6">
+        <v>43203</v>
+      </c>
       <c r="C132" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D132" s="3">
-        <v>4</v>
+      <c r="D132" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="14"/>
       <c r="G132" s="3"/>
     </row>
-    <row r="133" spans="3:7">
+    <row r="133" spans="2:7">
+      <c r="B133" s="6">
+        <v>43203</v>
+      </c>
       <c r="C133" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D133" s="3"/>
+      <c r="D133" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E133" s="3"/>
       <c r="F133" s="14"/>
       <c r="G133" s="3"/>
     </row>
-    <row r="134" spans="3:7">
+    <row r="134" spans="2:7">
+      <c r="B134" s="6">
+        <v>43203</v>
+      </c>
       <c r="C134" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="D134" s="3"/>
+      <c r="D134" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="E134" s="3"/>
       <c r="F134" s="14"/>
       <c r="G134" s="3"/>
     </row>
-    <row r="136" spans="3:7">
+    <row r="136" spans="2:7">
+      <c r="B136" s="6">
+        <v>43203</v>
+      </c>
       <c r="C136" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D136" s="3"/>
+      <c r="D136" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E136" s="3"/>
       <c r="F136" s="14"/>
       <c r="G136" s="3"/>
     </row>
-    <row r="137" spans="3:7">
+    <row r="137" spans="2:7">
+      <c r="B137" s="6">
+        <v>43203</v>
+      </c>
       <c r="C137" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D137" s="3"/>
+      <c r="D137" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E137" s="3"/>
       <c r="F137" s="14"/>
       <c r="G137" s="3"/>
     </row>
-    <row r="138" spans="3:7">
+    <row r="138" spans="2:7">
+      <c r="B138" s="6">
+        <v>43203</v>
+      </c>
       <c r="C138" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D138" s="3"/>
+      <c r="D138" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E138" s="3"/>
       <c r="F138" s="14"/>
       <c r="G138" s="3"/>
     </row>
-    <row r="139" spans="3:7">
+    <row r="139" spans="2:7">
+      <c r="B139" s="6">
+        <v>43203</v>
+      </c>
       <c r="C139" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D139" s="3"/>
+      <c r="D139" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E139" s="3"/>
       <c r="F139" s="14"/>
       <c r="G139" s="3"/>
     </row>
-    <row r="140" spans="3:7">
+    <row r="140" spans="2:7">
+      <c r="B140" s="6">
+        <v>43203</v>
+      </c>
       <c r="C140" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D140" s="3"/>
+      <c r="D140" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E140" s="3"/>
       <c r="F140" s="14"/>
       <c r="G140" s="3"/>
     </row>
-    <row r="141" spans="3:7">
+    <row r="141" spans="2:7">
+      <c r="B141" s="6">
+        <v>43203</v>
+      </c>
       <c r="C141" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D141" s="3"/>
+      <c r="D141" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E141" s="3"/>
       <c r="F141" s="14"/>
       <c r="G141" s="3"/>
     </row>
-    <row r="142" spans="3:7">
+    <row r="142" spans="2:7">
+      <c r="B142" s="6">
+        <v>43203</v>
+      </c>
       <c r="C142" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D142" s="3">
-        <v>5</v>
+      <c r="D142" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="E142" s="3"/>
       <c r="F142" s="14"/>
       <c r="G142" s="3"/>
     </row>
-    <row r="143" spans="3:7">
+    <row r="143" spans="2:7">
+      <c r="B143" s="6">
+        <v>43203</v>
+      </c>
       <c r="C143" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D143" s="3"/>
+      <c r="D143" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E143" s="3"/>
       <c r="F143" s="14"/>
       <c r="G143" s="3"/>
     </row>
-    <row r="144" spans="3:7">
+    <row r="144" spans="2:7">
+      <c r="B144" s="6">
+        <v>43203</v>
+      </c>
       <c r="C144" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D144" s="3"/>
+      <c r="D144" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E144" s="3"/>
       <c r="F144" s="14"/>
       <c r="G144" s="3"/>
     </row>
-    <row r="145" spans="3:7">
+    <row r="145" spans="2:7">
+      <c r="B145" s="6">
+        <v>43203</v>
+      </c>
       <c r="C145" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D145" s="3"/>
+      <c r="D145" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E145" s="3"/>
       <c r="F145" s="14"/>
       <c r="G145" s="3"/>
     </row>
-    <row r="146" spans="3:7">
+    <row r="146" spans="2:7">
+      <c r="B146" s="6">
+        <v>43203</v>
+      </c>
       <c r="C146" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D146" s="3"/>
+      <c r="D146" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E146" s="3"/>
       <c r="F146" s="14"/>
       <c r="G146" s="3"/>
     </row>
-    <row r="147" spans="3:7">
+    <row r="147" spans="2:7">
+      <c r="B147" s="6">
+        <v>43203</v>
+      </c>
       <c r="C147" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D147" s="3"/>
+      <c r="D147" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E147" s="3"/>
       <c r="F147" s="14"/>
       <c r="G147" s="3"/>
     </row>
-    <row r="148" spans="3:7">
+    <row r="148" spans="2:7">
+      <c r="B148" s="6">
+        <v>43203</v>
+      </c>
       <c r="C148" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D148" s="3"/>
+      <c r="D148" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E148" s="3"/>
       <c r="F148" s="14"/>
       <c r="G148" s="3"/>
     </row>
-    <row r="149" spans="3:7">
+    <row r="149" spans="2:7">
+      <c r="B149" s="6">
+        <v>43203</v>
+      </c>
       <c r="C149" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D149" s="3"/>
+      <c r="D149" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E149" s="3"/>
       <c r="F149" s="14"/>
       <c r="G149" s="3"/>
     </row>
-    <row r="150" spans="3:7">
+    <row r="150" spans="2:7">
+      <c r="B150" s="6">
+        <v>43203</v>
+      </c>
       <c r="C150" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="D150" s="3"/>
+      <c r="D150" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="E150" s="3"/>
       <c r="F150" s="14"/>
       <c r="G150" s="3"/>
     </row>
-    <row r="151" spans="3:7">
+    <row r="151" spans="2:7">
+      <c r="B151" s="6">
+        <v>43203</v>
+      </c>
       <c r="C151" s="3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="152" spans="3:7">
+      <c r="D151" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7">
+      <c r="B152" s="6">
+        <v>43203</v>
+      </c>
       <c r="C152" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="153" spans="3:7">
+      <c r="D152" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7">
+      <c r="B153" s="6">
+        <v>43203</v>
+      </c>
       <c r="C153" s="3" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="154" spans="3:7">
+      <c r="D153" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7">
+      <c r="B154" s="6">
+        <v>43203</v>
+      </c>
       <c r="C154" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="155" spans="3:7">
+      <c r="D154" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7">
+      <c r="B155" s="6">
+        <v>43203</v>
+      </c>
       <c r="C155" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="156" spans="3:7">
+      <c r="D155" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7">
+      <c r="B156" s="6">
+        <v>43203</v>
+      </c>
       <c r="C156" s="3" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="157" spans="3:7">
+      <c r="D156" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7">
+      <c r="B157" s="6">
+        <v>43203</v>
+      </c>
       <c r="C157" s="3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="158" spans="3:7">
+      <c r="D157" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7">
+      <c r="B158" s="6">
+        <v>43203</v>
+      </c>
       <c r="C158" s="3" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="159" spans="3:7">
+      <c r="D158" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7">
+      <c r="B159" s="6">
+        <v>43203</v>
+      </c>
       <c r="C159" s="3" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="160" spans="3:7">
+      <c r="D159" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7">
+      <c r="B160" s="6">
+        <v>43203</v>
+      </c>
       <c r="C160" s="3" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="161" spans="3:3">
+      <c r="D160" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4">
+      <c r="B161" s="6">
+        <v>43203</v>
+      </c>
       <c r="C161" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="162" spans="3:3">
+      <c r="D161" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4">
+      <c r="B162" s="6">
+        <v>43203</v>
+      </c>
       <c r="C162" s="3" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="163" spans="3:3">
+      <c r="D162" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4">
+      <c r="B163" s="6">
+        <v>43203</v>
+      </c>
       <c r="C163" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="164" spans="3:3">
+      <c r="D163" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4">
+      <c r="B164" s="6">
+        <v>43203</v>
+      </c>
       <c r="C164" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="165" spans="3:3">
+      <c r="D164" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4">
+      <c r="B165" s="6">
+        <v>43203</v>
+      </c>
       <c r="C165" s="3" t="s">
         <v>160</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3955,9 +4276,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <pane xSplit="11440" topLeftCell="J1" activePane="topRight"/>
-      <selection activeCell="B33" sqref="B33"/>
-      <selection pane="topRight" activeCell="F11" sqref="F11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5131,12 +5450,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="I11:I13"/>
     <mergeCell ref="I35:I37"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="I20:I22"/>
@@ -5144,6 +5457,12 @@
     <mergeCell ref="I26:I28"/>
     <mergeCell ref="I29:I31"/>
     <mergeCell ref="I32:I34"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="I11:I13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>